<commit_message>
updated validation statistics for new variable names
</commit_message>
<xml_diff>
--- a/input/validation_statistics.xlsx
+++ b/input/validation_statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\andy_local\SimPaths project files\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F6FBF4-91CC-447F-913C-0BFC0D603513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24E245B6-B2F1-4310-87E4-5617F0D1B145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="839" firstSheet="43" activeTab="44" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="839" firstSheet="43" activeTab="46" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IT_studentsByAge" sheetId="26" r:id="rId1"/>
@@ -57,9 +57,9 @@
     <sheet name="UK_hourlywageByGenderAndEdu" sheetId="23" r:id="rId42"/>
     <sheet name="UK_lhwByGenderAndEdu" sheetId="24" r:id="rId43"/>
     <sheet name="UK_lhwByGender" sheetId="25" r:id="rId44"/>
-    <sheet name="UK_mentalWellbeingByAgeGroup" sheetId="53" r:id="rId45"/>
-    <sheet name="UK_physicalWellbeingByAgeGroup" sheetId="54" r:id="rId46"/>
-    <sheet name="UK_lifeSatisfactionByAgeGroup" sheetId="55" r:id="rId47"/>
+    <sheet name="UK_lifeSatisfactionByAgeGroup" sheetId="56" r:id="rId45"/>
+    <sheet name="UK_healthMCSByAgeGroup" sheetId="57" r:id="rId46"/>
+    <sheet name="UK_healthPCSByAgeGroup" sheetId="58" r:id="rId47"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -845,114 +845,6 @@
     <t>employed_female_ITC</t>
   </si>
   <si>
-    <t>mental_wellbeing_male_80_100</t>
-  </si>
-  <si>
-    <t>mental_wellbeing_female_80_100</t>
-  </si>
-  <si>
-    <t>mental_wellbeing_male_70_79</t>
-  </si>
-  <si>
-    <t>mental_wellbeing_female_70_79</t>
-  </si>
-  <si>
-    <t>mental_wellbeing_male_60_69</t>
-  </si>
-  <si>
-    <t>mental_wellbeing_female_60_69</t>
-  </si>
-  <si>
-    <t>mental_wellbeing_male_50_59</t>
-  </si>
-  <si>
-    <t>mental_wellbeing_female_50_59</t>
-  </si>
-  <si>
-    <t>mental_wellbeing_male_40_49</t>
-  </si>
-  <si>
-    <t>mental_wellbeing_female_40_49</t>
-  </si>
-  <si>
-    <t>mental_wellbeing_male_30_39</t>
-  </si>
-  <si>
-    <t>mental_wellbeing_female_30_39</t>
-  </si>
-  <si>
-    <t>mental_wellbeing_male_20_29</t>
-  </si>
-  <si>
-    <t>mental_wellbeing_female_20_29</t>
-  </si>
-  <si>
-    <t>mental_wellbeing_male_10_19</t>
-  </si>
-  <si>
-    <t>mental_wellbeing_female_10_19</t>
-  </si>
-  <si>
-    <t>mental_wellbeing_male_0_9</t>
-  </si>
-  <si>
-    <t>mental_wellbeing_female_0_9</t>
-  </si>
-  <si>
-    <t>physical_wellbeing_male_80_100</t>
-  </si>
-  <si>
-    <t>physical_wellbeing_female_80_100</t>
-  </si>
-  <si>
-    <t>physical_wellbeing_male_70_79</t>
-  </si>
-  <si>
-    <t>physical_wellbeing_female_70_79</t>
-  </si>
-  <si>
-    <t>physical_wellbeing_male_60_69</t>
-  </si>
-  <si>
-    <t>physical_wellbeing_female_60_69</t>
-  </si>
-  <si>
-    <t>physical_wellbeing_male_50_59</t>
-  </si>
-  <si>
-    <t>physical_wellbeing_female_50_59</t>
-  </si>
-  <si>
-    <t>physical_wellbeing_male_40_49</t>
-  </si>
-  <si>
-    <t>physical_wellbeing_female_40_49</t>
-  </si>
-  <si>
-    <t>physical_wellbeing_male_30_39</t>
-  </si>
-  <si>
-    <t>physical_wellbeing_female_30_39</t>
-  </si>
-  <si>
-    <t>physical_wellbeing_male_20_29</t>
-  </si>
-  <si>
-    <t>physical_wellbeing_female_20_29</t>
-  </si>
-  <si>
-    <t>physical_wellbeing_male_10_19</t>
-  </si>
-  <si>
-    <t>physical_wellbeing_female_10_19</t>
-  </si>
-  <si>
-    <t>physical_wellbeing_male_0_9</t>
-  </si>
-  <si>
-    <t>physical_wellbeing_female_0_9</t>
-  </si>
-  <si>
     <t>life_satisfaction_male_80_100</t>
   </si>
   <si>
@@ -1005,6 +897,114 @@
   </si>
   <si>
     <t>life_satisfaction_female_0_9</t>
+  </si>
+  <si>
+    <t>health_mcs_score_female_0_9</t>
+  </si>
+  <si>
+    <t>health_mcs_score_male_0_9</t>
+  </si>
+  <si>
+    <t>health_mcs_score_female_10_19</t>
+  </si>
+  <si>
+    <t>health_mcs_score_male_10_19</t>
+  </si>
+  <si>
+    <t>health_mcs_score_female_20_29</t>
+  </si>
+  <si>
+    <t>health_mcs_score_male_20_29</t>
+  </si>
+  <si>
+    <t>health_mcs_score_female_30_39</t>
+  </si>
+  <si>
+    <t>health_mcs_score_male_30_39</t>
+  </si>
+  <si>
+    <t>health_mcs_score_female_40_49</t>
+  </si>
+  <si>
+    <t>health_mcs_score_male_40_49</t>
+  </si>
+  <si>
+    <t>health_mcs_score_female_50_59</t>
+  </si>
+  <si>
+    <t>health_mcs_score_male_50_59</t>
+  </si>
+  <si>
+    <t>health_mcs_score_female_60_69</t>
+  </si>
+  <si>
+    <t>health_mcs_score_male_60_69</t>
+  </si>
+  <si>
+    <t>health_mcs_score_female_70_79</t>
+  </si>
+  <si>
+    <t>health_mcs_score_male_70_79</t>
+  </si>
+  <si>
+    <t>health_mcs_score_female_80_100</t>
+  </si>
+  <si>
+    <t>health_mcs_score_male_80_100</t>
+  </si>
+  <si>
+    <t>health_pcs_score_female_0_9</t>
+  </si>
+  <si>
+    <t>health_pcs_score_male_0_9</t>
+  </si>
+  <si>
+    <t>health_pcs_score_female_10_19</t>
+  </si>
+  <si>
+    <t>health_pcs_score_male_10_19</t>
+  </si>
+  <si>
+    <t>health_pcs_score_female_20_29</t>
+  </si>
+  <si>
+    <t>health_pcs_score_male_20_29</t>
+  </si>
+  <si>
+    <t>health_pcs_score_female_30_39</t>
+  </si>
+  <si>
+    <t>health_pcs_score_male_30_39</t>
+  </si>
+  <si>
+    <t>health_pcs_score_female_40_49</t>
+  </si>
+  <si>
+    <t>health_pcs_score_male_40_49</t>
+  </si>
+  <si>
+    <t>health_pcs_score_female_50_59</t>
+  </si>
+  <si>
+    <t>health_pcs_score_male_50_59</t>
+  </si>
+  <si>
+    <t>health_pcs_score_female_60_69</t>
+  </si>
+  <si>
+    <t>health_pcs_score_male_60_69</t>
+  </si>
+  <si>
+    <t>health_pcs_score_female_70_79</t>
+  </si>
+  <si>
+    <t>health_pcs_score_male_70_79</t>
+  </si>
+  <si>
+    <t>health_pcs_score_female_80_100</t>
+  </si>
+  <si>
+    <t>health_pcs_score_male_80_100</t>
   </si>
 </sst>
 </file>
@@ -16874,16 +16874,14 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D46F2A-ADE4-40DC-94AC-D12894191FA4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6110EFEF-5A01-4DCE-A763-CA975C41B28B}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -16950,58 +16948,58 @@
         <v>2022</v>
       </c>
       <c r="B2" s="3">
-        <v>42.387451171875</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3">
-        <v>44.138294219970703</v>
+        <v>5</v>
       </c>
       <c r="D2" s="3">
-        <v>41.773311614990227</v>
+        <v>4.9473670815003112</v>
       </c>
       <c r="E2" s="3">
-        <v>46.542930603027337</v>
+        <v>5.1040844640421081</v>
       </c>
       <c r="F2" s="3">
-        <v>42.777542114257813</v>
+        <v>5.0333282040384653</v>
       </c>
       <c r="G2" s="3">
-        <v>45.389362335205078</v>
+        <v>4.9030890916881713</v>
       </c>
       <c r="H2" s="3">
-        <v>42.801361083984382</v>
+        <v>4.9900372659891943</v>
       </c>
       <c r="I2" s="3">
-        <v>44.521034240722663</v>
+        <v>4.9532779135865628</v>
       </c>
       <c r="J2" s="3">
-        <v>44.823432922363281</v>
+        <v>5.0075712359057611</v>
       </c>
       <c r="K2" s="3">
-        <v>47.540950775146477</v>
+        <v>5.0862687149237997</v>
       </c>
       <c r="L2" s="3">
-        <v>46.129112243652337</v>
+        <v>4.9263923865663068</v>
       </c>
       <c r="M2" s="3">
-        <v>48.322052001953132</v>
+        <v>4.9954649101296829</v>
       </c>
       <c r="N2" s="3">
-        <v>48.231998443603523</v>
+        <v>5.1447935051748477</v>
       </c>
       <c r="O2" s="3">
-        <v>50.792964935302727</v>
+        <v>5.3392897410776232</v>
       </c>
       <c r="P2" s="3">
-        <v>50.347324371337891</v>
+        <v>5.564984983723992</v>
       </c>
       <c r="Q2" s="3">
-        <v>51.371414184570313</v>
+        <v>5.4003840827709606</v>
       </c>
       <c r="R2" s="3">
-        <v>52.547672271728523</v>
+        <v>5.6573521253079377</v>
       </c>
       <c r="S2" s="3">
-        <v>52.209869384765632</v>
+        <v>5.5216762931784897</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -17009,58 +17007,58 @@
         <v>2021</v>
       </c>
       <c r="B3" s="3">
-        <v>42.464492797851563</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3">
-        <v>44.225425720214837</v>
+        <v>5</v>
       </c>
       <c r="D3" s="3">
-        <v>41.502498626708977</v>
+        <v>4.9613212208943827</v>
       </c>
       <c r="E3" s="3">
-        <v>45.820247650146477</v>
+        <v>5.1095008113228877</v>
       </c>
       <c r="F3" s="3">
-        <v>40.829277038574219</v>
+        <v>5.0123925533412779</v>
       </c>
       <c r="G3" s="3">
-        <v>45.226459503173828</v>
+        <v>5.0301418339485693</v>
       </c>
       <c r="H3" s="3">
-        <v>43.081333160400391</v>
+        <v>5.0787445570875986</v>
       </c>
       <c r="I3" s="3">
-        <v>45.626583099365227</v>
+        <v>5.0471906266071578</v>
       </c>
       <c r="J3" s="3">
-        <v>44.675117492675781</v>
+        <v>4.9784911518287362</v>
       </c>
       <c r="K3" s="3">
-        <v>47.128021240234382</v>
+        <v>5.0527937191611896</v>
       </c>
       <c r="L3" s="3">
-        <v>46.531475067138672</v>
+        <v>4.9908818102540433</v>
       </c>
       <c r="M3" s="3">
-        <v>48.790843963623047</v>
+        <v>5.0700889811441261</v>
       </c>
       <c r="N3" s="3">
-        <v>48.466297149658203</v>
+        <v>5.1871266846892086</v>
       </c>
       <c r="O3" s="3">
-        <v>50.670406341552727</v>
+        <v>5.2664446748759062</v>
       </c>
       <c r="P3" s="3">
-        <v>50.229526519775391</v>
+        <v>5.4727455892632184</v>
       </c>
       <c r="Q3" s="3">
-        <v>52.412921905517578</v>
+        <v>5.5764862351364766</v>
       </c>
       <c r="R3" s="3">
-        <v>51.560600280761719</v>
+        <v>5.637319399278085</v>
       </c>
       <c r="S3" s="3">
-        <v>52.971828460693359</v>
+        <v>5.6706813648229328</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -17068,58 +17066,58 @@
         <v>2020</v>
       </c>
       <c r="B4" s="3">
-        <v>42.664321899414063</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3">
-        <v>44.545307159423828</v>
+        <v>5</v>
       </c>
       <c r="D4" s="3">
-        <v>41.80731201171875</v>
+        <v>4.9934442297436279</v>
       </c>
       <c r="E4" s="3">
-        <v>45.706317901611328</v>
+        <v>5.1199360069467383</v>
       </c>
       <c r="F4" s="3">
-        <v>41.42010498046875</v>
+        <v>5.0158787280590316</v>
       </c>
       <c r="G4" s="3">
-        <v>46.223026275634773</v>
+        <v>5.1020334320990806</v>
       </c>
       <c r="H4" s="3">
-        <v>43.092498779296882</v>
+        <v>5.1417166005043313</v>
       </c>
       <c r="I4" s="3">
-        <v>45.494724273681641</v>
+        <v>5.0629601510096327</v>
       </c>
       <c r="J4" s="3">
-        <v>44.639095306396477</v>
+        <v>4.9839173070781886</v>
       </c>
       <c r="K4" s="3">
-        <v>47.779186248779297</v>
+        <v>5.0653189584942906</v>
       </c>
       <c r="L4" s="3">
-        <v>46.091636657714837</v>
+        <v>4.9514677314738416</v>
       </c>
       <c r="M4" s="3">
-        <v>48.839241027832031</v>
+        <v>5.0755392121389864</v>
       </c>
       <c r="N4" s="3">
-        <v>48.523162841796882</v>
+        <v>5.2737492321617294</v>
       </c>
       <c r="O4" s="3">
-        <v>50.550708770751953</v>
+        <v>5.3052365966802766</v>
       </c>
       <c r="P4" s="3">
-        <v>50.376853942871087</v>
+        <v>5.5530234865234531</v>
       </c>
       <c r="Q4" s="3">
-        <v>52.596214294433587</v>
+        <v>5.6119841864645847</v>
       </c>
       <c r="R4" s="3">
-        <v>51.528499603271477</v>
+        <v>5.6535603285214906</v>
       </c>
       <c r="S4" s="3">
-        <v>52.607730865478523</v>
+        <v>5.659220700227019</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -17127,58 +17125,58 @@
         <v>2019</v>
       </c>
       <c r="B5" s="3">
-        <v>43.006427764892578</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3">
-        <v>45.047077178955078</v>
+        <v>5</v>
       </c>
       <c r="D5" s="3">
-        <v>43.05828857421875</v>
+        <v>4.9815058035494406</v>
       </c>
       <c r="E5" s="3">
-        <v>46.407253265380859</v>
+        <v>5.0800824937637499</v>
       </c>
       <c r="F5" s="3">
-        <v>42.579074859619141</v>
+        <v>5.0785856645403253</v>
       </c>
       <c r="G5" s="3">
-        <v>45.897056579589837</v>
+        <v>5.0306921075521798</v>
       </c>
       <c r="H5" s="3">
-        <v>44.115150451660163</v>
+        <v>5.0693314156142453</v>
       </c>
       <c r="I5" s="3">
-        <v>46.258148193359382</v>
+        <v>5.0260162923848952</v>
       </c>
       <c r="J5" s="3">
-        <v>45.964481353759773</v>
+        <v>4.9552083912161073</v>
       </c>
       <c r="K5" s="3">
-        <v>47.645378112792969</v>
+        <v>4.9866281814126356</v>
       </c>
       <c r="L5" s="3">
-        <v>47.048931121826172</v>
+        <v>4.9102675836177587</v>
       </c>
       <c r="M5" s="3">
-        <v>48.816165924072273</v>
+        <v>5.0076816238901456</v>
       </c>
       <c r="N5" s="3">
-        <v>49.311569213867188</v>
+        <v>5.2200884992539054</v>
       </c>
       <c r="O5" s="3">
-        <v>51.040512084960938</v>
+        <v>5.2579645682358072</v>
       </c>
       <c r="P5" s="3">
-        <v>50.98089599609375</v>
+        <v>5.4554878539910181</v>
       </c>
       <c r="Q5" s="3">
-        <v>52.598297119140632</v>
+        <v>5.5325465575076791</v>
       </c>
       <c r="R5" s="3">
-        <v>51.121086120605469</v>
+        <v>5.5180624594266359</v>
       </c>
       <c r="S5" s="3">
-        <v>52.270164489746087</v>
+        <v>5.4820374721529914</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -17186,58 +17184,58 @@
         <v>2018</v>
       </c>
       <c r="B6" s="3">
-        <v>43.528789520263672</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3">
-        <v>45.598335266113281</v>
+        <v>5</v>
       </c>
       <c r="D6" s="3">
-        <v>43.051609039306641</v>
+        <v>4.9654016268823069</v>
       </c>
       <c r="E6" s="3">
-        <v>46.533378601074219</v>
+        <v>5.0951873253109863</v>
       </c>
       <c r="F6" s="3">
-        <v>43.325119018554688</v>
+        <v>5.0597276811824976</v>
       </c>
       <c r="G6" s="3">
-        <v>46.716567993164063</v>
+        <v>5.0164525245646896</v>
       </c>
       <c r="H6" s="3">
-        <v>44.469741821289063</v>
+        <v>5.0498170502262143</v>
       </c>
       <c r="I6" s="3">
-        <v>47.040962219238281</v>
+        <v>5.0234953453249123</v>
       </c>
       <c r="J6" s="3">
-        <v>46.249324798583977</v>
+        <v>4.9786177855940954</v>
       </c>
       <c r="K6" s="3">
-        <v>48.147380828857422</v>
+        <v>5.0032311237537526</v>
       </c>
       <c r="L6" s="3">
-        <v>47.264247894287109</v>
+        <v>4.9474697827293479</v>
       </c>
       <c r="M6" s="3">
-        <v>49.248821258544922</v>
+        <v>5.010858783762683</v>
       </c>
       <c r="N6" s="3">
-        <v>49.614063262939453</v>
+        <v>5.2404017907079066</v>
       </c>
       <c r="O6" s="3">
-        <v>51.520000457763672</v>
+        <v>5.2816701538328106</v>
       </c>
       <c r="P6" s="3">
-        <v>51.231700897216797</v>
+        <v>5.4960577905424346</v>
       </c>
       <c r="Q6" s="3">
-        <v>52.843494415283203</v>
+        <v>5.5361494179142046</v>
       </c>
       <c r="R6" s="3">
-        <v>51.668491363525391</v>
+        <v>5.6349959629476958</v>
       </c>
       <c r="S6" s="3">
-        <v>52.250984191894531</v>
+        <v>5.5945908998065192</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -17245,58 +17243,58 @@
         <v>2017</v>
       </c>
       <c r="B7" s="3">
-        <v>43.937515258789063</v>
+        <v>5</v>
       </c>
       <c r="C7" s="3">
-        <v>45.944019317626953</v>
+        <v>5</v>
       </c>
       <c r="D7" s="3">
-        <v>44.056625366210938</v>
+        <v>5.0181585209855486</v>
       </c>
       <c r="E7" s="3">
-        <v>47.493152618408203</v>
+        <v>5.1718471947531901</v>
       </c>
       <c r="F7" s="3">
-        <v>44.851455688476563</v>
+        <v>5.1596076851408856</v>
       </c>
       <c r="G7" s="3">
-        <v>47.250133514404297</v>
+        <v>5.1066017555767829</v>
       </c>
       <c r="H7" s="3">
-        <v>45.527545928955078</v>
+        <v>5.1037393310224877</v>
       </c>
       <c r="I7" s="3">
-        <v>47.323085784912109</v>
+        <v>5.1234941679568253</v>
       </c>
       <c r="J7" s="3">
-        <v>46.480400085449219</v>
+        <v>4.9873293532844221</v>
       </c>
       <c r="K7" s="3">
-        <v>48.528656005859382</v>
+        <v>5.0144566825019652</v>
       </c>
       <c r="L7" s="3">
-        <v>47.686687469482422</v>
+        <v>4.9925647355767024</v>
       </c>
       <c r="M7" s="3">
-        <v>49.764095306396477</v>
+        <v>5.0365709112652883</v>
       </c>
       <c r="N7" s="3">
-        <v>50.100063323974609</v>
+        <v>5.3058251598264494</v>
       </c>
       <c r="O7" s="3">
-        <v>51.623218536376953</v>
+        <v>5.3232571718954276</v>
       </c>
       <c r="P7" s="3">
-        <v>51.365566253662109</v>
+        <v>5.5378859501006898</v>
       </c>
       <c r="Q7" s="3">
-        <v>52.657535552978523</v>
+        <v>5.4951247475517997</v>
       </c>
       <c r="R7" s="3">
-        <v>51.558723449707031</v>
+        <v>5.5338439891927802</v>
       </c>
       <c r="S7" s="3">
-        <v>52.871547698974609</v>
+        <v>5.4576808937696262</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -17304,58 +17302,58 @@
         <v>2016</v>
       </c>
       <c r="B8" s="3">
-        <v>44.147449493408203</v>
+        <v>5</v>
       </c>
       <c r="C8" s="3">
-        <v>46.029079437255859</v>
+        <v>5</v>
       </c>
       <c r="D8" s="3">
-        <v>44.656585693359382</v>
+        <v>5.091956714643378</v>
       </c>
       <c r="E8" s="3">
-        <v>48.037738800048828</v>
+        <v>5.1979045277818718</v>
       </c>
       <c r="F8" s="3">
-        <v>45.530742645263672</v>
+        <v>5.2042124879998202</v>
       </c>
       <c r="G8" s="3">
-        <v>47.789054870605469</v>
+        <v>5.1261608958290177</v>
       </c>
       <c r="H8" s="3">
-        <v>46.032386779785163</v>
+        <v>5.1757579794255868</v>
       </c>
       <c r="I8" s="3">
-        <v>48.224277496337891</v>
+        <v>5.1646315233332949</v>
       </c>
       <c r="J8" s="3">
-        <v>47.059951782226563</v>
+        <v>5.072366768255014</v>
       </c>
       <c r="K8" s="3">
-        <v>49.284721374511719</v>
+        <v>5.2336913369683877</v>
       </c>
       <c r="L8" s="3">
-        <v>48.048797607421882</v>
+        <v>5.0609537838680998</v>
       </c>
       <c r="M8" s="3">
-        <v>50.215641021728523</v>
+        <v>5.1514258032878733</v>
       </c>
       <c r="N8" s="3">
-        <v>50.592567443847663</v>
+        <v>5.3805427063853628</v>
       </c>
       <c r="O8" s="3">
-        <v>51.894119262695313</v>
+        <v>5.3578744924364248</v>
       </c>
       <c r="P8" s="3">
-        <v>51.295646667480469</v>
+        <v>5.5048935874882794</v>
       </c>
       <c r="Q8" s="3">
-        <v>52.906242370605469</v>
+        <v>5.5980584175023624</v>
       </c>
       <c r="R8" s="3">
-        <v>51.442481994628913</v>
+        <v>5.6329869947111044</v>
       </c>
       <c r="S8" s="3">
-        <v>52.317516326904297</v>
+        <v>5.525797385452389</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -17363,58 +17361,58 @@
         <v>2015</v>
       </c>
       <c r="B9" s="3">
-        <v>44.439807891845703</v>
+        <v>5</v>
       </c>
       <c r="C9" s="3">
-        <v>46.2977294921875</v>
+        <v>5</v>
       </c>
       <c r="D9" s="3">
-        <v>45.366226196289063</v>
+        <v>5.1161207081428888</v>
       </c>
       <c r="E9" s="3">
-        <v>48.363872528076172</v>
+        <v>5.1586791710112356</v>
       </c>
       <c r="F9" s="3">
-        <v>46.203872680664063</v>
+        <v>5.2322350720679003</v>
       </c>
       <c r="G9" s="3">
-        <v>48.353851318359382</v>
+        <v>5.0832157211609754</v>
       </c>
       <c r="H9" s="3">
-        <v>46.653354644775391</v>
+        <v>5.2577953512742202</v>
       </c>
       <c r="I9" s="3">
-        <v>48.780078887939453</v>
+        <v>5.156980686444613</v>
       </c>
       <c r="J9" s="3">
-        <v>47.505771636962891</v>
+        <v>5.1187839229182117</v>
       </c>
       <c r="K9" s="3">
-        <v>49.854881286621087</v>
+        <v>5.2070515266428181</v>
       </c>
       <c r="L9" s="3">
-        <v>48.053680419921882</v>
+        <v>5.0712504208004123</v>
       </c>
       <c r="M9" s="3">
-        <v>50.858325958251953</v>
+        <v>5.205072319555919</v>
       </c>
       <c r="N9" s="3">
-        <v>50.734916687011719</v>
+        <v>5.4061642306260991</v>
       </c>
       <c r="O9" s="3">
-        <v>52.473155975341797</v>
+        <v>5.4122209526646357</v>
       </c>
       <c r="P9" s="3">
-        <v>51.905036926269531</v>
+        <v>5.6075850567044698</v>
       </c>
       <c r="Q9" s="3">
-        <v>53.512557983398438</v>
+        <v>5.5589451975493267</v>
       </c>
       <c r="R9" s="3">
-        <v>51.883296966552727</v>
+        <v>5.6058398265117271</v>
       </c>
       <c r="S9" s="3">
-        <v>52.835803985595703</v>
+        <v>5.5649840715378822</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -17422,58 +17420,58 @@
         <v>2014</v>
       </c>
       <c r="B10" s="3">
-        <v>44.681266784667969</v>
+        <v>5</v>
       </c>
       <c r="C10" s="3">
-        <v>46.560455322265632</v>
+        <v>5</v>
       </c>
       <c r="D10" s="3">
-        <v>45.583587646484382</v>
+        <v>5.0764589583984776</v>
       </c>
       <c r="E10" s="3">
-        <v>48.157482147216797</v>
+        <v>5.1371618670971477</v>
       </c>
       <c r="F10" s="3">
-        <v>46.286861419677727</v>
+        <v>5.1415114541260714</v>
       </c>
       <c r="G10" s="3">
-        <v>48.749351501464837</v>
+        <v>5.0393908872109749</v>
       </c>
       <c r="H10" s="3">
-        <v>47.231494903564453</v>
+        <v>5.1301997611431061</v>
       </c>
       <c r="I10" s="3">
-        <v>49.204944610595703</v>
+        <v>5.1695715747398694</v>
       </c>
       <c r="J10" s="3">
-        <v>48.063453674316413</v>
+        <v>5.0132614581149566</v>
       </c>
       <c r="K10" s="3">
-        <v>50.217250823974609</v>
+        <v>5.0950120107390138</v>
       </c>
       <c r="L10" s="3">
-        <v>48.425819396972663</v>
+        <v>5.0081136352843769</v>
       </c>
       <c r="M10" s="3">
-        <v>50.665378570556641</v>
+        <v>5.0053232542660089</v>
       </c>
       <c r="N10" s="3">
-        <v>50.984184265136719</v>
+        <v>5.2406530729039131</v>
       </c>
       <c r="O10" s="3">
-        <v>52.671157836914063</v>
+        <v>5.2637436520297092</v>
       </c>
       <c r="P10" s="3">
-        <v>52.060153961181641</v>
+        <v>5.4207346222576103</v>
       </c>
       <c r="Q10" s="3">
-        <v>53.378032684326172</v>
+        <v>5.366055383274233</v>
       </c>
       <c r="R10" s="3">
-        <v>52.068271636962891</v>
+        <v>5.412244371410142</v>
       </c>
       <c r="S10" s="3">
-        <v>52.859161376953132</v>
+        <v>5.3903643381577249</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -17481,58 +17479,58 @@
         <v>2013</v>
       </c>
       <c r="B11" s="3">
-        <v>44.542011260986328</v>
+        <v>5</v>
       </c>
       <c r="C11" s="3">
-        <v>46.530723571777337</v>
+        <v>5</v>
       </c>
       <c r="D11" s="3">
-        <v>45.480381011962891</v>
+        <v>5.0269010706692763</v>
       </c>
       <c r="E11" s="3">
-        <v>48.116680145263672</v>
+        <v>5.1348274908599354</v>
       </c>
       <c r="F11" s="3">
-        <v>46.768203735351563</v>
+        <v>5.0735101031514391</v>
       </c>
       <c r="G11" s="3">
-        <v>48.865737915039063</v>
+        <v>5.013711248729372</v>
       </c>
       <c r="H11" s="3">
-        <v>46.942195892333977</v>
+        <v>5.0312839818835444</v>
       </c>
       <c r="I11" s="3">
-        <v>49.304145812988281</v>
+        <v>5.0187757957899093</v>
       </c>
       <c r="J11" s="3">
-        <v>47.680217742919922</v>
+        <v>4.8780584621308751</v>
       </c>
       <c r="K11" s="3">
-        <v>49.762992858886719</v>
+        <v>4.912059750537578</v>
       </c>
       <c r="L11" s="3">
-        <v>48.166309356689453</v>
+        <v>4.782507941384158</v>
       </c>
       <c r="M11" s="3">
-        <v>50.470344543457031</v>
+        <v>4.8404125767247228</v>
       </c>
       <c r="N11" s="3">
-        <v>51.053909301757813</v>
+        <v>5.2115792323504992</v>
       </c>
       <c r="O11" s="3">
-        <v>52.711021423339837</v>
+        <v>5.231789563674754</v>
       </c>
       <c r="P11" s="3">
-        <v>51.55072021484375</v>
+        <v>5.2659253126512509</v>
       </c>
       <c r="Q11" s="3">
-        <v>53.088176727294922</v>
+        <v>5.2849310471579436</v>
       </c>
       <c r="R11" s="3">
-        <v>51.747634887695313</v>
+        <v>5.2209533631997944</v>
       </c>
       <c r="S11" s="3">
-        <v>53.680828094482422</v>
+        <v>5.274529490219324</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -17540,58 +17538,58 @@
         <v>2012</v>
       </c>
       <c r="B12" s="3">
-        <v>44.591228485107422</v>
+        <v>5</v>
       </c>
       <c r="C12" s="3">
-        <v>46.644489288330078</v>
+        <v>5</v>
       </c>
       <c r="D12" s="3">
-        <v>45.696113586425781</v>
+        <v>5.0308304616237063</v>
       </c>
       <c r="E12" s="3">
-        <v>48.027179718017578</v>
+        <v>5.1090067791443943</v>
       </c>
       <c r="F12" s="3">
-        <v>46.350143432617188</v>
+        <v>5.0794961760364954</v>
       </c>
       <c r="G12" s="3">
-        <v>48.964859008789063</v>
+        <v>5.0289939318549708</v>
       </c>
       <c r="H12" s="3">
-        <v>47.316696166992188</v>
+        <v>5.1014296287027738</v>
       </c>
       <c r="I12" s="3">
-        <v>49.640903472900391</v>
+        <v>5.0318479219292476</v>
       </c>
       <c r="J12" s="3">
-        <v>47.746620178222663</v>
+        <v>4.9400838483586043</v>
       </c>
       <c r="K12" s="3">
-        <v>49.926887512207031</v>
+        <v>4.9464984353218124</v>
       </c>
       <c r="L12" s="3">
-        <v>48.280540466308587</v>
+        <v>4.911621954964656</v>
       </c>
       <c r="M12" s="3">
-        <v>50.946426391601563</v>
+        <v>4.9646400874541063</v>
       </c>
       <c r="N12" s="3">
-        <v>51.256732940673828</v>
+        <v>5.3228031139371224</v>
       </c>
       <c r="O12" s="3">
-        <v>53.064353942871087</v>
+        <v>5.2921515435831052</v>
       </c>
       <c r="P12" s="3">
-        <v>51.669384002685547</v>
+        <v>5.3400803544434332</v>
       </c>
       <c r="Q12" s="3">
-        <v>53.517246246337891</v>
+        <v>5.3663605222657997</v>
       </c>
       <c r="R12" s="3">
-        <v>51.562103271484382</v>
+        <v>5.2207790839758994</v>
       </c>
       <c r="S12" s="3">
-        <v>53.278205871582031</v>
+        <v>5.3171145739591719</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -17599,58 +17597,58 @@
         <v>2011</v>
       </c>
       <c r="B13" s="3">
-        <v>44.961589813232422</v>
+        <v>5</v>
       </c>
       <c r="C13" s="3">
-        <v>46.929721832275391</v>
+        <v>5</v>
       </c>
       <c r="D13" s="3">
-        <v>46.246410369873047</v>
+        <v>5.1176851247528212</v>
       </c>
       <c r="E13" s="3">
-        <v>48.508377075195313</v>
+        <v>5.1671432816770348</v>
       </c>
       <c r="F13" s="3">
-        <v>47.381927490234382</v>
+        <v>5.1569093627650764</v>
       </c>
       <c r="G13" s="3">
-        <v>49.610820770263672</v>
+        <v>5.1183831664895942</v>
       </c>
       <c r="H13" s="3">
-        <v>47.78106689453125</v>
+        <v>5.0922362798196943</v>
       </c>
       <c r="I13" s="3">
-        <v>49.748382568359382</v>
+        <v>5.0810507047778053</v>
       </c>
       <c r="J13" s="3">
-        <v>48.493812561035163</v>
+        <v>4.9971914506053681</v>
       </c>
       <c r="K13" s="3">
-        <v>50.381671905517578</v>
+        <v>5.0848699512533857</v>
       </c>
       <c r="L13" s="3">
-        <v>48.701705932617188</v>
+        <v>5.0091007177902966</v>
       </c>
       <c r="M13" s="3">
-        <v>50.987308502197273</v>
+        <v>5.0797028974482403</v>
       </c>
       <c r="N13" s="3">
-        <v>51.295967102050781</v>
+        <v>5.3715733788656959</v>
       </c>
       <c r="O13" s="3">
-        <v>52.735763549804688</v>
+        <v>5.343952981175339</v>
       </c>
       <c r="P13" s="3">
-        <v>51.528736114501953</v>
+        <v>5.4784648453319207</v>
       </c>
       <c r="Q13" s="3">
-        <v>53.291397094726563</v>
+        <v>5.4776614581525056</v>
       </c>
       <c r="R13" s="3">
-        <v>51.948570251464837</v>
+        <v>5.3830223159770894</v>
       </c>
       <c r="S13" s="3">
-        <v>53.622611999511719</v>
+        <v>5.4919357866675567</v>
       </c>
     </row>
   </sheetData>
@@ -17659,16 +17657,14 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{415930B8-0E96-4054-856F-1518B1E6B997}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EDB3B34-E005-4C87-B8C9-18F31BE8EBDE}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -17676,58 +17672,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -17735,58 +17731,58 @@
         <v>2022</v>
       </c>
       <c r="B2" s="3">
-        <v>61.320938110351563</v>
+        <v>42.387932395771813</v>
       </c>
       <c r="C2" s="3">
-        <v>61.86737060546875</v>
+        <v>44.138288521782243</v>
       </c>
       <c r="D2" s="3">
-        <v>56.764640808105469</v>
+        <v>41.773307197990981</v>
       </c>
       <c r="E2" s="3">
-        <v>57.880725860595703</v>
+        <v>46.542943401439921</v>
       </c>
       <c r="F2" s="3">
-        <v>53.984916687011719</v>
+        <v>42.777534136271512</v>
       </c>
       <c r="G2" s="3">
-        <v>54.047801971435547</v>
+        <v>45.389405052402829</v>
       </c>
       <c r="H2" s="3">
-        <v>52.138229370117188</v>
+        <v>42.801475275462103</v>
       </c>
       <c r="I2" s="3">
-        <v>54.058082580566413</v>
+        <v>44.521091951445648</v>
       </c>
       <c r="J2" s="3">
-        <v>49.586513519287109</v>
+        <v>44.823522520167373</v>
       </c>
       <c r="K2" s="3">
-        <v>51.540542602539063</v>
+        <v>47.541100806181348</v>
       </c>
       <c r="L2" s="3">
-        <v>47.673286437988281</v>
+        <v>46.129113843686198</v>
       </c>
       <c r="M2" s="3">
-        <v>49.951545715332031</v>
+        <v>48.322070178801177</v>
       </c>
       <c r="N2" s="3">
-        <v>45.927528381347663</v>
+        <v>48.232054546044942</v>
       </c>
       <c r="O2" s="3">
-        <v>46.966922760009773</v>
+        <v>50.792932958267123</v>
       </c>
       <c r="P2" s="3">
-        <v>44.300556182861328</v>
+        <v>50.347353923552127</v>
       </c>
       <c r="Q2" s="3">
-        <v>45.473728179931641</v>
+        <v>51.371380455976599</v>
       </c>
       <c r="R2" s="3">
-        <v>36.218776702880859</v>
+        <v>52.547699544956672</v>
       </c>
       <c r="S2" s="3">
-        <v>40.600582122802727</v>
+        <v>52.209875546611748</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -17794,58 +17790,58 @@
         <v>2021</v>
       </c>
       <c r="B3" s="3">
-        <v>61.357151031494141</v>
+        <v>42.464496033292257</v>
       </c>
       <c r="C3" s="3">
-        <v>61.902900695800781</v>
+        <v>44.225424703842492</v>
       </c>
       <c r="D3" s="3">
-        <v>57.133205413818359</v>
+        <v>41.502513861235428</v>
       </c>
       <c r="E3" s="3">
-        <v>58.298576354980469</v>
+        <v>45.820091774316211</v>
       </c>
       <c r="F3" s="3">
-        <v>54.861289978027337</v>
+        <v>40.829191259345258</v>
       </c>
       <c r="G3" s="3">
-        <v>55.313266754150391</v>
+        <v>45.226492817854457</v>
       </c>
       <c r="H3" s="3">
-        <v>52.791030883789063</v>
+        <v>43.081382047195113</v>
       </c>
       <c r="I3" s="3">
-        <v>54.132244110107422</v>
+        <v>45.626545613685067</v>
       </c>
       <c r="J3" s="3">
-        <v>51.187171936035163</v>
+        <v>44.675078684324831</v>
       </c>
       <c r="K3" s="3">
-        <v>52.2227783203125</v>
+        <v>47.128095649974242</v>
       </c>
       <c r="L3" s="3">
-        <v>48.547214508056641</v>
+        <v>46.531513209736858</v>
       </c>
       <c r="M3" s="3">
-        <v>49.866989135742188</v>
+        <v>48.790862004833748</v>
       </c>
       <c r="N3" s="3">
-        <v>46.639926910400391</v>
+        <v>48.466301065923417</v>
       </c>
       <c r="O3" s="3">
-        <v>47.25714111328125</v>
+        <v>50.670435496496793</v>
       </c>
       <c r="P3" s="3">
-        <v>43.904552459716797</v>
+        <v>50.229495650873609</v>
       </c>
       <c r="Q3" s="3">
-        <v>44.943393707275391</v>
+        <v>52.4129361430739</v>
       </c>
       <c r="R3" s="3">
-        <v>36.722373962402337</v>
+        <v>51.560535747375177</v>
       </c>
       <c r="S3" s="3">
-        <v>41.054515838623047</v>
+        <v>52.971874522853781</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -17853,58 +17849,58 @@
         <v>2020</v>
       </c>
       <c r="B4" s="3">
-        <v>61.341869354248047</v>
+        <v>42.664327248462897</v>
       </c>
       <c r="C4" s="3">
-        <v>61.80035400390625</v>
+        <v>44.54530229454452</v>
       </c>
       <c r="D4" s="3">
-        <v>57.616466522216797</v>
+        <v>41.807293336803973</v>
       </c>
       <c r="E4" s="3">
-        <v>58.036636352539063</v>
+        <v>45.70625623649115</v>
       </c>
       <c r="F4" s="3">
-        <v>54.661056518554688</v>
+        <v>41.420042049533713</v>
       </c>
       <c r="G4" s="3">
-        <v>55.141170501708977</v>
+        <v>46.222960821502632</v>
       </c>
       <c r="H4" s="3">
-        <v>53.432815551757813</v>
+        <v>43.092662753102132</v>
       </c>
       <c r="I4" s="3">
-        <v>54.61517333984375</v>
+        <v>45.494703092555277</v>
       </c>
       <c r="J4" s="3">
-        <v>51.066738128662109</v>
+        <v>44.639196202321664</v>
       </c>
       <c r="K4" s="3">
-        <v>52.452651977539063</v>
+        <v>47.779246242625788</v>
       </c>
       <c r="L4" s="3">
-        <v>48.485126495361328</v>
+        <v>46.091694328398653</v>
       </c>
       <c r="M4" s="3">
-        <v>49.993869781494141</v>
+        <v>48.839218166202699</v>
       </c>
       <c r="N4" s="3">
-        <v>46.651607513427727</v>
+        <v>48.523156481090467</v>
       </c>
       <c r="O4" s="3">
-        <v>46.948795318603523</v>
+        <v>50.550717763173807</v>
       </c>
       <c r="P4" s="3">
-        <v>43.263458251953132</v>
+        <v>50.37686646006577</v>
       </c>
       <c r="Q4" s="3">
-        <v>44.892196655273438</v>
+        <v>52.596218539254231</v>
       </c>
       <c r="R4" s="3">
-        <v>37.387798309326172</v>
+        <v>51.528419025308743</v>
       </c>
       <c r="S4" s="3">
-        <v>39.843677520751953</v>
+        <v>52.607787299207757</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -17912,58 +17908,58 @@
         <v>2019</v>
       </c>
       <c r="B5" s="3">
-        <v>60.941165924072273</v>
+        <v>43.006434440124359</v>
       </c>
       <c r="C5" s="3">
-        <v>61.473960876464837</v>
+        <v>45.047069465022062</v>
       </c>
       <c r="D5" s="3">
-        <v>57.007221221923828</v>
+        <v>43.058389214666398</v>
       </c>
       <c r="E5" s="3">
-        <v>57.357086181640632</v>
+        <v>46.407244269732537</v>
       </c>
       <c r="F5" s="3">
-        <v>54.553138732910163</v>
+        <v>42.574386139931292</v>
       </c>
       <c r="G5" s="3">
-        <v>55.378273010253913</v>
+        <v>45.896448302684988</v>
       </c>
       <c r="H5" s="3">
-        <v>52.110828399658203</v>
+        <v>44.115234792169574</v>
       </c>
       <c r="I5" s="3">
-        <v>53.98870849609375</v>
+        <v>46.258173661457427</v>
       </c>
       <c r="J5" s="3">
-        <v>50.758190155029297</v>
+        <v>45.964596037775287</v>
       </c>
       <c r="K5" s="3">
-        <v>52.143760681152337</v>
+        <v>47.645333075612527</v>
       </c>
       <c r="L5" s="3">
-        <v>48.494773864746087</v>
+        <v>47.048959422028908</v>
       </c>
       <c r="M5" s="3">
-        <v>49.72747802734375</v>
+        <v>48.816186699032208</v>
       </c>
       <c r="N5" s="3">
-        <v>46.065288543701172</v>
+        <v>49.31153919037672</v>
       </c>
       <c r="O5" s="3">
-        <v>46.636478424072273</v>
+        <v>51.040581438438643</v>
       </c>
       <c r="P5" s="3">
-        <v>43.037395477294922</v>
+        <v>50.980881872742877</v>
       </c>
       <c r="Q5" s="3">
-        <v>45.38623046875</v>
+        <v>52.598341383166087</v>
       </c>
       <c r="R5" s="3">
-        <v>38.426731109619141</v>
+        <v>51.121015599843822</v>
       </c>
       <c r="S5" s="3">
-        <v>40.319957733154297</v>
+        <v>52.270196693878312</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -17971,58 +17967,58 @@
         <v>2018</v>
       </c>
       <c r="B6" s="3">
-        <v>60.635910034179688</v>
+        <v>43.529125662451079</v>
       </c>
       <c r="C6" s="3">
-        <v>61.24835205078125</v>
+        <v>45.59834374594341</v>
       </c>
       <c r="D6" s="3">
-        <v>56.911190032958977</v>
+        <v>43.051482483468327</v>
       </c>
       <c r="E6" s="3">
-        <v>57.274772644042969</v>
+        <v>46.533378572133067</v>
       </c>
       <c r="F6" s="3">
-        <v>54.498401641845703</v>
+        <v>43.329103229042254</v>
       </c>
       <c r="G6" s="3">
-        <v>55.390933990478523</v>
+        <v>46.717118204810383</v>
       </c>
       <c r="H6" s="3">
-        <v>52.744289398193359</v>
+        <v>44.469032141982808</v>
       </c>
       <c r="I6" s="3">
-        <v>54.390392303466797</v>
+        <v>47.045121607523079</v>
       </c>
       <c r="J6" s="3">
-        <v>50.7354736328125</v>
+        <v>46.249414344467382</v>
       </c>
       <c r="K6" s="3">
-        <v>52.270843505859382</v>
+        <v>48.147328468818387</v>
       </c>
       <c r="L6" s="3">
-        <v>48.404060363769531</v>
+        <v>47.264286837860098</v>
       </c>
       <c r="M6" s="3">
-        <v>49.860027313232422</v>
+        <v>49.248939040415827</v>
       </c>
       <c r="N6" s="3">
-        <v>45.739669799804688</v>
+        <v>49.611796012418637</v>
       </c>
       <c r="O6" s="3">
-        <v>47.172248840332031</v>
+        <v>51.519424742256867</v>
       </c>
       <c r="P6" s="3">
-        <v>43.511516571044922</v>
+        <v>51.231645125806502</v>
       </c>
       <c r="Q6" s="3">
-        <v>44.997066497802727</v>
+        <v>52.843593660276568</v>
       </c>
       <c r="R6" s="3">
-        <v>38.156982421875</v>
+        <v>51.668324186088249</v>
       </c>
       <c r="S6" s="3">
-        <v>40.266620635986328</v>
+        <v>52.2509479274391</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -18030,58 +18026,58 @@
         <v>2017</v>
       </c>
       <c r="B7" s="3">
-        <v>60.629802703857422</v>
+        <v>43.937505160864127</v>
       </c>
       <c r="C7" s="3">
-        <v>61.125526428222663</v>
+        <v>45.94402125910198</v>
       </c>
       <c r="D7" s="3">
-        <v>56.690467834472663</v>
+        <v>44.056619984096621</v>
       </c>
       <c r="E7" s="3">
-        <v>57.354488372802727</v>
+        <v>47.49306860895809</v>
       </c>
       <c r="F7" s="3">
-        <v>54.427024841308587</v>
+        <v>44.848755037985832</v>
       </c>
       <c r="G7" s="3">
-        <v>55.5135498046875</v>
+        <v>47.250134016471158</v>
       </c>
       <c r="H7" s="3">
-        <v>52.934391021728523</v>
+        <v>45.527634810511238</v>
       </c>
       <c r="I7" s="3">
-        <v>54.368152618408203</v>
+        <v>47.307872058276708</v>
       </c>
       <c r="J7" s="3">
-        <v>50.886966705322273</v>
+        <v>46.4804220920212</v>
       </c>
       <c r="K7" s="3">
-        <v>52.123401641845703</v>
+        <v>48.528704182879359</v>
       </c>
       <c r="L7" s="3">
-        <v>48.494636535644531</v>
+        <v>47.686701428742538</v>
       </c>
       <c r="M7" s="3">
-        <v>49.213775634765632</v>
+        <v>49.764110630171068</v>
       </c>
       <c r="N7" s="3">
-        <v>45.925975799560547</v>
+        <v>50.097950226771012</v>
       </c>
       <c r="O7" s="3">
-        <v>46.761077880859382</v>
+        <v>51.622395651330933</v>
       </c>
       <c r="P7" s="3">
-        <v>43.097080230712891</v>
+        <v>51.3655028210338</v>
       </c>
       <c r="Q7" s="3">
-        <v>44.723548889160163</v>
+        <v>52.65759678376844</v>
       </c>
       <c r="R7" s="3">
-        <v>37.488559722900391</v>
+        <v>51.558809788628842</v>
       </c>
       <c r="S7" s="3">
-        <v>39.418842315673828</v>
+        <v>52.871498867811447</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -18089,58 +18085,58 @@
         <v>2016</v>
       </c>
       <c r="B8" s="3">
-        <v>60.353588104248047</v>
+        <v>44.147445654864747</v>
       </c>
       <c r="C8" s="3">
-        <v>60.954612731933587</v>
+        <v>46.029077244037452</v>
       </c>
       <c r="D8" s="3">
-        <v>57.094913482666023</v>
+        <v>44.656633106362932</v>
       </c>
       <c r="E8" s="3">
-        <v>57.564891815185547</v>
+        <v>48.037692329313643</v>
       </c>
       <c r="F8" s="3">
-        <v>54.331073760986328</v>
+        <v>45.535307215444753</v>
       </c>
       <c r="G8" s="3">
-        <v>55.504413604736328</v>
+        <v>47.812651970088297</v>
       </c>
       <c r="H8" s="3">
-        <v>53.077156066894531</v>
+        <v>46.032549647892452</v>
       </c>
       <c r="I8" s="3">
-        <v>54.483345031738281</v>
+        <v>48.223330696476609</v>
       </c>
       <c r="J8" s="3">
-        <v>50.990619659423828</v>
+        <v>47.060051959350957</v>
       </c>
       <c r="K8" s="3">
-        <v>52.750911712646477</v>
+        <v>49.284716792966861</v>
       </c>
       <c r="L8" s="3">
-        <v>48.542713165283203</v>
+        <v>48.048785001043747</v>
       </c>
       <c r="M8" s="3">
-        <v>49.605884552001953</v>
+        <v>50.215713067347707</v>
       </c>
       <c r="N8" s="3">
-        <v>46.142585754394531</v>
+        <v>50.592566764768883</v>
       </c>
       <c r="O8" s="3">
-        <v>47.128181457519531</v>
+        <v>51.894057739941317</v>
       </c>
       <c r="P8" s="3">
-        <v>42.450729370117188</v>
+        <v>51.29564878630535</v>
       </c>
       <c r="Q8" s="3">
-        <v>44.397636413574219</v>
+        <v>52.906243023153188</v>
       </c>
       <c r="R8" s="3">
-        <v>37.524478912353523</v>
+        <v>51.442533076120291</v>
       </c>
       <c r="S8" s="3">
-        <v>39.849155426025391</v>
+        <v>52.317513309095908</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -18148,58 +18144,58 @@
         <v>2015</v>
       </c>
       <c r="B9" s="3">
-        <v>60.138576507568359</v>
+        <v>44.439814869756127</v>
       </c>
       <c r="C9" s="3">
-        <v>60.642356872558587</v>
+        <v>46.297600937837203</v>
       </c>
       <c r="D9" s="3">
-        <v>56.895565032958977</v>
+        <v>45.366196851037273</v>
       </c>
       <c r="E9" s="3">
-        <v>57.597274780273438</v>
+        <v>48.363838392564688</v>
       </c>
       <c r="F9" s="3">
-        <v>54.601325988769531</v>
+        <v>46.203452804171043</v>
       </c>
       <c r="G9" s="3">
-        <v>55.858798980712891</v>
+        <v>48.354172831788482</v>
       </c>
       <c r="H9" s="3">
-        <v>53.070205688476563</v>
+        <v>46.653392208242813</v>
       </c>
       <c r="I9" s="3">
-        <v>54.320461273193359</v>
+        <v>48.780592775721637</v>
       </c>
       <c r="J9" s="3">
-        <v>51.19744873046875</v>
+        <v>47.505806676354538</v>
       </c>
       <c r="K9" s="3">
-        <v>52.645427703857422</v>
+        <v>49.854920056439937</v>
       </c>
       <c r="L9" s="3">
-        <v>48.720466613769531</v>
+        <v>48.053648285114548</v>
       </c>
       <c r="M9" s="3">
-        <v>50.198539733886719</v>
+        <v>50.858326168693459</v>
       </c>
       <c r="N9" s="3">
-        <v>46.091876983642578</v>
+        <v>50.734927396152912</v>
       </c>
       <c r="O9" s="3">
-        <v>47.225780487060547</v>
+        <v>52.473127122016407</v>
       </c>
       <c r="P9" s="3">
-        <v>42.994800567626953</v>
+        <v>51.905041049588633</v>
       </c>
       <c r="Q9" s="3">
-        <v>44.304752349853523</v>
+        <v>53.512632035519587</v>
       </c>
       <c r="R9" s="3">
-        <v>37.893363952636719</v>
+        <v>51.883297169569147</v>
       </c>
       <c r="S9" s="3">
-        <v>39.352165222167969</v>
+        <v>52.835801726962899</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -18207,58 +18203,58 @@
         <v>2014</v>
       </c>
       <c r="B10" s="3">
-        <v>59.831611633300781</v>
+        <v>44.681266024181546</v>
       </c>
       <c r="C10" s="3">
-        <v>60.408233642578132</v>
+        <v>46.560294737720042</v>
       </c>
       <c r="D10" s="3">
-        <v>56.547573089599609</v>
+        <v>45.583670127318257</v>
       </c>
       <c r="E10" s="3">
-        <v>57.108402252197273</v>
+        <v>48.157520392592041</v>
       </c>
       <c r="F10" s="3">
-        <v>54.33062744140625</v>
+        <v>46.287988042391802</v>
       </c>
       <c r="G10" s="3">
-        <v>55.550434112548828</v>
+        <v>48.746008167841723</v>
       </c>
       <c r="H10" s="3">
-        <v>53.149078369140632</v>
+        <v>47.231488748230028</v>
       </c>
       <c r="I10" s="3">
-        <v>54.25677490234375</v>
+        <v>49.205504873377137</v>
       </c>
       <c r="J10" s="3">
-        <v>51.353828430175781</v>
+        <v>48.06338307526741</v>
       </c>
       <c r="K10" s="3">
-        <v>52.632476806640632</v>
+        <v>50.217244317996602</v>
       </c>
       <c r="L10" s="3">
-        <v>48.7745361328125</v>
+        <v>48.425787893396922</v>
       </c>
       <c r="M10" s="3">
-        <v>50.066207885742188</v>
+        <v>50.66533178265005</v>
       </c>
       <c r="N10" s="3">
-        <v>45.950756072998047</v>
+        <v>50.984123961689512</v>
       </c>
       <c r="O10" s="3">
-        <v>46.729000091552727</v>
+        <v>52.671143169602168</v>
       </c>
       <c r="P10" s="3">
-        <v>42.637096405029297</v>
+        <v>52.059981177263737</v>
       </c>
       <c r="Q10" s="3">
-        <v>43.902847290039063</v>
+        <v>53.378006501791127</v>
       </c>
       <c r="R10" s="3">
-        <v>37.365325927734382</v>
+        <v>52.068218410787189</v>
       </c>
       <c r="S10" s="3">
-        <v>39.519218444824219</v>
+        <v>52.859142460492649</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -18266,58 +18262,58 @@
         <v>2013</v>
       </c>
       <c r="B11" s="3">
-        <v>59.783512115478523</v>
+        <v>44.542020120314547</v>
       </c>
       <c r="C11" s="3">
-        <v>60.437183380126953</v>
+        <v>46.530975791210373</v>
       </c>
       <c r="D11" s="3">
-        <v>56.820384979248047</v>
+        <v>45.474999507306428</v>
       </c>
       <c r="E11" s="3">
-        <v>57.150241851806641</v>
+        <v>48.116704974877038</v>
       </c>
       <c r="F11" s="3">
-        <v>54.336235046386719</v>
+        <v>46.769707805973567</v>
       </c>
       <c r="G11" s="3">
-        <v>55.236717224121087</v>
+        <v>48.859659902286559</v>
       </c>
       <c r="H11" s="3">
-        <v>53.472213745117188</v>
+        <v>46.941636462130333</v>
       </c>
       <c r="I11" s="3">
-        <v>54.317760467529297</v>
+        <v>49.3036768597471</v>
       </c>
       <c r="J11" s="3">
-        <v>51.485328674316413</v>
+        <v>47.680287420579518</v>
       </c>
       <c r="K11" s="3">
-        <v>52.754413604736328</v>
+        <v>49.763054201837072</v>
       </c>
       <c r="L11" s="3">
-        <v>49.000946044921882</v>
+        <v>48.166320573784937</v>
       </c>
       <c r="M11" s="3">
-        <v>50.0062255859375</v>
+        <v>50.470337390291071</v>
       </c>
       <c r="N11" s="3">
-        <v>46.05816650390625</v>
+        <v>51.053922971664498</v>
       </c>
       <c r="O11" s="3">
-        <v>47.232616424560547</v>
+        <v>52.710970851844358</v>
       </c>
       <c r="P11" s="3">
-        <v>42.413303375244141</v>
+        <v>51.550802084984781</v>
       </c>
       <c r="Q11" s="3">
-        <v>43.549098968505859</v>
+        <v>53.08815107068704</v>
       </c>
       <c r="R11" s="3">
-        <v>37.631690979003913</v>
+        <v>51.74764864150584</v>
       </c>
       <c r="S11" s="3">
-        <v>40.401626586914063</v>
+        <v>53.680865849140467</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -18325,58 +18321,58 @@
         <v>2012</v>
       </c>
       <c r="B12" s="3">
-        <v>59.720111846923828</v>
+        <v>44.591236272660048</v>
       </c>
       <c r="C12" s="3">
-        <v>60.426155090332031</v>
+        <v>46.644496096770759</v>
       </c>
       <c r="D12" s="3">
-        <v>56.287807464599609</v>
+        <v>45.69556029409825</v>
       </c>
       <c r="E12" s="3">
-        <v>57.025497436523438</v>
+        <v>48.027714825779938</v>
       </c>
       <c r="F12" s="3">
-        <v>54.129344940185547</v>
+        <v>46.346896048571068</v>
       </c>
       <c r="G12" s="3">
-        <v>55.176044464111328</v>
+        <v>48.964676610131711</v>
       </c>
       <c r="H12" s="3">
-        <v>53.2730712890625</v>
+        <v>47.316753700880533</v>
       </c>
       <c r="I12" s="3">
-        <v>54.08087158203125</v>
+        <v>49.646826377060798</v>
       </c>
       <c r="J12" s="3">
-        <v>51.67816162109375</v>
+        <v>47.74657483065922</v>
       </c>
       <c r="K12" s="3">
-        <v>52.6834716796875</v>
+        <v>49.926951069883778</v>
       </c>
       <c r="L12" s="3">
-        <v>49.025928497314453</v>
+        <v>48.28048046816204</v>
       </c>
       <c r="M12" s="3">
-        <v>50.358840942382813</v>
+        <v>50.94644357265252</v>
       </c>
       <c r="N12" s="3">
-        <v>46.343540191650391</v>
+        <v>51.256791372488621</v>
       </c>
       <c r="O12" s="3">
-        <v>46.997592926025391</v>
+        <v>53.06433202168656</v>
       </c>
       <c r="P12" s="3">
-        <v>42.311611175537109</v>
+        <v>51.669341662263001</v>
       </c>
       <c r="Q12" s="3">
-        <v>44.079715728759773</v>
+        <v>53.517222965794552</v>
       </c>
       <c r="R12" s="3">
-        <v>38.154148101806641</v>
+        <v>51.562034680086761</v>
       </c>
       <c r="S12" s="3">
-        <v>40.839572906494141</v>
+        <v>53.278209520200839</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -18384,58 +18380,58 @@
         <v>2011</v>
       </c>
       <c r="B13" s="3">
-        <v>59.668697357177727</v>
+        <v>44.961598280175913</v>
       </c>
       <c r="C13" s="3">
-        <v>60.491851806640632</v>
+        <v>46.929734834477777</v>
       </c>
       <c r="D13" s="3">
-        <v>56.433101654052727</v>
+        <v>46.246464861618051</v>
       </c>
       <c r="E13" s="3">
-        <v>57.157581329345703</v>
+        <v>48.508359773925093</v>
       </c>
       <c r="F13" s="3">
-        <v>54.436279296875</v>
+        <v>47.381383476146119</v>
       </c>
       <c r="G13" s="3">
-        <v>55.391872406005859</v>
+        <v>49.612984607556193</v>
       </c>
       <c r="H13" s="3">
-        <v>53.513195037841797</v>
+        <v>47.781103558979012</v>
       </c>
       <c r="I13" s="3">
-        <v>54.441608428955078</v>
+        <v>49.748321519986668</v>
       </c>
       <c r="J13" s="3">
-        <v>51.604328155517578</v>
+        <v>48.493845970320727</v>
       </c>
       <c r="K13" s="3">
-        <v>52.69293212890625</v>
+        <v>50.381672934926883</v>
       </c>
       <c r="L13" s="3">
-        <v>48.823509216308587</v>
+        <v>48.701679532754753</v>
       </c>
       <c r="M13" s="3">
-        <v>49.98272705078125</v>
+        <v>50.987328315529247</v>
       </c>
       <c r="N13" s="3">
-        <v>46.147701263427727</v>
+        <v>51.295903211173098</v>
       </c>
       <c r="O13" s="3">
-        <v>46.895244598388672</v>
+        <v>52.735782735604822</v>
       </c>
       <c r="P13" s="3">
-        <v>42.085227966308587</v>
+        <v>51.528728700040439</v>
       </c>
       <c r="Q13" s="3">
-        <v>43.141876220703132</v>
+        <v>53.291376624384448</v>
       </c>
       <c r="R13" s="3">
-        <v>37.575214385986328</v>
+        <v>51.948619429818677</v>
       </c>
       <c r="S13" s="3">
-        <v>40.297603607177727</v>
+        <v>53.622609313269479</v>
       </c>
     </row>
   </sheetData>
@@ -18444,16 +18440,14 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE1505B-0907-4DD3-8CE0-6A19323D9FCC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4DC31E3-0F92-41AC-A9AE-B4DDD81986B7}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.85546875" style="2"/>
+    <col min="1" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -18461,58 +18455,58 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>296</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -18520,58 +18514,58 @@
         <v>2022</v>
       </c>
       <c r="B2" s="3">
-        <v>5</v>
+        <v>61.321330893104722</v>
       </c>
       <c r="C2" s="3">
-        <v>5</v>
+        <v>61.867377507998633</v>
       </c>
       <c r="D2" s="3">
-        <v>4.9473719596862793</v>
+        <v>56.764586675448697</v>
       </c>
       <c r="E2" s="3">
-        <v>5.1040773391723633</v>
+        <v>57.880819762251633</v>
       </c>
       <c r="F2" s="3">
-        <v>5.0333285331726074</v>
+        <v>53.984943883071587</v>
       </c>
       <c r="G2" s="3">
-        <v>4.9030866622924796</v>
+        <v>54.047871288023558</v>
       </c>
       <c r="H2" s="3">
-        <v>4.9900093078613281</v>
+        <v>52.138438618660018</v>
       </c>
       <c r="I2" s="3">
-        <v>4.9532608985900879</v>
+        <v>54.058104611712473</v>
       </c>
       <c r="J2" s="3">
-        <v>5.0075592994689941</v>
+        <v>49.586578727808757</v>
       </c>
       <c r="K2" s="3">
-        <v>5.0862445831298828</v>
+        <v>51.540627438195791</v>
       </c>
       <c r="L2" s="3">
-        <v>4.9263806343078613</v>
+        <v>47.673338993140653</v>
       </c>
       <c r="M2" s="3">
-        <v>4.9954662322998047</v>
+        <v>49.951567523232093</v>
       </c>
       <c r="N2" s="3">
-        <v>5.1447882652282706</v>
+        <v>45.927564889526089</v>
       </c>
       <c r="O2" s="3">
-        <v>5.3392915725708008</v>
+        <v>46.966873931872037</v>
       </c>
       <c r="P2" s="3">
-        <v>5.5649838447570801</v>
+        <v>44.300520229199797</v>
       </c>
       <c r="Q2" s="3">
-        <v>5.4003915786743164</v>
+        <v>45.473690233874208</v>
       </c>
       <c r="R2" s="3">
-        <v>5.6573681831359863</v>
+        <v>36.21869549469784</v>
       </c>
       <c r="S2" s="3">
-        <v>5.5216817855834961</v>
+        <v>40.600546266142317</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -18579,58 +18573,58 @@
         <v>2021</v>
       </c>
       <c r="B3" s="3">
-        <v>5</v>
+        <v>61.357144096633377</v>
       </c>
       <c r="C3" s="3">
-        <v>5</v>
+        <v>61.902901058911553</v>
       </c>
       <c r="D3" s="3">
-        <v>4.9613280296325684</v>
+        <v>57.133249886669127</v>
       </c>
       <c r="E3" s="3">
-        <v>5.1095113754272461</v>
+        <v>58.298727631147919</v>
       </c>
       <c r="F3" s="3">
-        <v>5.0123934745788574</v>
+        <v>54.86131107074052</v>
       </c>
       <c r="G3" s="3">
-        <v>5.0301470756530762</v>
+        <v>55.313257724363012</v>
       </c>
       <c r="H3" s="3">
-        <v>5.0787181854248047</v>
+        <v>52.791064121641469</v>
       </c>
       <c r="I3" s="3">
-        <v>5.0471830368041992</v>
+        <v>54.132243653702332</v>
       </c>
       <c r="J3" s="3">
-        <v>4.9784932136535636</v>
+        <v>51.187332885673847</v>
       </c>
       <c r="K3" s="3">
-        <v>5.0527796745300293</v>
+        <v>52.222830827730739</v>
       </c>
       <c r="L3" s="3">
-        <v>4.990872859954834</v>
+        <v>48.547236445764852</v>
       </c>
       <c r="M3" s="3">
-        <v>5.0700855255126953</v>
+        <v>49.867040256528419</v>
       </c>
       <c r="N3" s="3">
-        <v>5.1871223449707031</v>
+        <v>46.639964365263431</v>
       </c>
       <c r="O3" s="3">
-        <v>5.2664370536804199</v>
+        <v>47.257184952541103</v>
       </c>
       <c r="P3" s="3">
-        <v>5.4727535247802734</v>
+        <v>43.904480006020847</v>
       </c>
       <c r="Q3" s="3">
-        <v>5.5764832496643066</v>
+        <v>44.943348444776582</v>
       </c>
       <c r="R3" s="3">
-        <v>5.637321949005127</v>
+        <v>36.722366022520013</v>
       </c>
       <c r="S3" s="3">
-        <v>5.6706743240356454</v>
+        <v>41.054562072107608</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -18638,58 +18632,58 @@
         <v>2020</v>
       </c>
       <c r="B4" s="3">
-        <v>5</v>
+        <v>61.341869578428103</v>
       </c>
       <c r="C4" s="3">
-        <v>5</v>
+        <v>61.800356131297121</v>
       </c>
       <c r="D4" s="3">
-        <v>4.9934501647949219</v>
+        <v>57.616410266410853</v>
       </c>
       <c r="E4" s="3">
-        <v>5.1199421882629386</v>
+        <v>58.036695513879359</v>
       </c>
       <c r="F4" s="3">
-        <v>5.0158896446228027</v>
+        <v>54.661116613150483</v>
       </c>
       <c r="G4" s="3">
-        <v>5.1020584106445313</v>
+        <v>55.141139837533188</v>
       </c>
       <c r="H4" s="3">
-        <v>5.141697883605957</v>
+        <v>53.432812061518433</v>
       </c>
       <c r="I4" s="3">
-        <v>5.0629544258117676</v>
+        <v>54.615179989521003</v>
       </c>
       <c r="J4" s="3">
-        <v>4.9838972091674796</v>
+        <v>51.066950654443268</v>
       </c>
       <c r="K4" s="3">
-        <v>5.0653061866760254</v>
+        <v>52.452657914254537</v>
       </c>
       <c r="L4" s="3">
-        <v>4.9514617919921884</v>
+        <v>48.485171909284418</v>
       </c>
       <c r="M4" s="3">
-        <v>5.0755467414855957</v>
+        <v>49.993935882030407</v>
       </c>
       <c r="N4" s="3">
-        <v>5.2737464904785156</v>
+        <v>46.651598263447632</v>
       </c>
       <c r="O4" s="3">
-        <v>5.3052272796630859</v>
+        <v>46.948861251379093</v>
       </c>
       <c r="P4" s="3">
-        <v>5.5530200004577637</v>
+        <v>43.263373054451137</v>
       </c>
       <c r="Q4" s="3">
-        <v>5.6119866371154794</v>
+        <v>44.892190777145153</v>
       </c>
       <c r="R4" s="3">
-        <v>5.6535654067993164</v>
+        <v>37.387707842379463</v>
       </c>
       <c r="S4" s="3">
-        <v>5.6592087745666504</v>
+        <v>39.843760440890513</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -18697,58 +18691,58 @@
         <v>2019</v>
       </c>
       <c r="B5" s="3">
-        <v>5</v>
+        <v>60.941166711149897</v>
       </c>
       <c r="C5" s="3">
-        <v>5</v>
+        <v>61.473966520686282</v>
       </c>
       <c r="D5" s="3">
-        <v>4.9815068244934082</v>
+        <v>57.007293502740957</v>
       </c>
       <c r="E5" s="3">
-        <v>5.0800743103027344</v>
+        <v>57.357188497609933</v>
       </c>
       <c r="F5" s="3">
-        <v>5.0789623260498047</v>
+        <v>54.551171899142638</v>
       </c>
       <c r="G5" s="3">
-        <v>5.0306816101074219</v>
+        <v>55.376297040667417</v>
       </c>
       <c r="H5" s="3">
-        <v>5.0693130493164063</v>
+        <v>52.110855684300297</v>
       </c>
       <c r="I5" s="3">
-        <v>5.0259957313537598</v>
+        <v>53.988717340536468</v>
       </c>
       <c r="J5" s="3">
-        <v>4.9551877975463867</v>
+        <v>50.75825033935849</v>
       </c>
       <c r="K5" s="3">
-        <v>4.9866271018981934</v>
+        <v>52.143815385104993</v>
       </c>
       <c r="L5" s="3">
-        <v>4.9102659225463867</v>
+        <v>48.494789468413792</v>
       </c>
       <c r="M5" s="3">
-        <v>5.0076727867126456</v>
+        <v>49.727577806226513</v>
       </c>
       <c r="N5" s="3">
-        <v>5.2200803756713867</v>
+        <v>46.06531349099977</v>
       </c>
       <c r="O5" s="3">
-        <v>5.257962703704834</v>
+        <v>46.636477672866441</v>
       </c>
       <c r="P5" s="3">
-        <v>5.4554810523986816</v>
+        <v>43.03746812475385</v>
       </c>
       <c r="Q5" s="3">
-        <v>5.5325474739074707</v>
+        <v>45.386180889894227</v>
       </c>
       <c r="R5" s="3">
-        <v>5.5180678367614746</v>
+        <v>38.426777416205297</v>
       </c>
       <c r="S5" s="3">
-        <v>5.4820337295532227</v>
+        <v>40.319883172604648</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -18756,58 +18750,58 @@
         <v>2018</v>
       </c>
       <c r="B6" s="3">
-        <v>5</v>
+        <v>60.635365785225559</v>
       </c>
       <c r="C6" s="3">
-        <v>5</v>
+        <v>61.248346908004009</v>
       </c>
       <c r="D6" s="3">
-        <v>4.9654035568237296</v>
+        <v>56.911311827093421</v>
       </c>
       <c r="E6" s="3">
-        <v>5.0951910018920898</v>
+        <v>57.274800716973843</v>
       </c>
       <c r="F6" s="3">
-        <v>5.0587320327758789</v>
+        <v>54.500671160666307</v>
       </c>
       <c r="G6" s="3">
-        <v>5.0164642333984384</v>
+        <v>55.39140846613649</v>
       </c>
       <c r="H6" s="3">
-        <v>5.0500755310058594</v>
+        <v>52.743263926108611</v>
       </c>
       <c r="I6" s="3">
-        <v>5.0216445922851563</v>
+        <v>54.389269693042003</v>
       </c>
       <c r="J6" s="3">
-        <v>4.978600025177002</v>
+        <v>50.735595742030547</v>
       </c>
       <c r="K6" s="3">
-        <v>5.00323486328125</v>
+        <v>52.271001932054723</v>
       </c>
       <c r="L6" s="3">
-        <v>4.9474616050720206</v>
+        <v>48.404105506162317</v>
       </c>
       <c r="M6" s="3">
-        <v>5.0108485221862793</v>
+        <v>49.86005623210206</v>
       </c>
       <c r="N6" s="3">
-        <v>5.2410998344421387</v>
+        <v>45.740170211708239</v>
       </c>
       <c r="O6" s="3">
-        <v>5.2824411392211914</v>
+        <v>47.17231879925842</v>
       </c>
       <c r="P6" s="3">
-        <v>5.4960641860961914</v>
+        <v>43.51141487979892</v>
       </c>
       <c r="Q6" s="3">
-        <v>5.5361232757568359</v>
+        <v>44.997207449490631</v>
       </c>
       <c r="R6" s="3">
-        <v>5.6349973678588867</v>
+        <v>38.157000646155517</v>
       </c>
       <c r="S6" s="3">
-        <v>5.5945882797241211</v>
+        <v>40.266696849462868</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -18815,58 +18809,58 @@
         <v>2017</v>
       </c>
       <c r="B7" s="3">
-        <v>5</v>
+        <v>60.629752510760397</v>
       </c>
       <c r="C7" s="3">
-        <v>5</v>
+        <v>61.125522940715257</v>
       </c>
       <c r="D7" s="3">
-        <v>5.0181612968444824</v>
+        <v>56.690444221483389</v>
       </c>
       <c r="E7" s="3">
-        <v>5.1718425750732422</v>
+        <v>57.354484872420883</v>
       </c>
       <c r="F7" s="3">
-        <v>5.1604361534118652</v>
+        <v>54.427171225602542</v>
       </c>
       <c r="G7" s="3">
-        <v>5.1066045761108398</v>
+        <v>55.513559482436293</v>
       </c>
       <c r="H7" s="3">
-        <v>5.1037302017211914</v>
+        <v>52.934495102443798</v>
       </c>
       <c r="I7" s="3">
-        <v>5.1249666213989258</v>
+        <v>54.375877321121713</v>
       </c>
       <c r="J7" s="3">
-        <v>4.9873228073120117</v>
+        <v>50.887068401880789</v>
       </c>
       <c r="K7" s="3">
-        <v>5.0144567489624023</v>
+        <v>52.123470590203937</v>
       </c>
       <c r="L7" s="3">
-        <v>4.9925661087036133</v>
+        <v>48.494663904676877</v>
       </c>
       <c r="M7" s="3">
-        <v>5.0365738868713379</v>
+        <v>49.213821455170859</v>
       </c>
       <c r="N7" s="3">
-        <v>5.3061652183532706</v>
+        <v>45.925983653848668</v>
       </c>
       <c r="O7" s="3">
-        <v>5.323634147644043</v>
+        <v>46.761543468884803</v>
       </c>
       <c r="P7" s="3">
-        <v>5.5378990173339844</v>
+        <v>43.097040644837953</v>
       </c>
       <c r="Q7" s="3">
-        <v>5.4951057434082031</v>
+        <v>44.723569855456873</v>
       </c>
       <c r="R7" s="3">
-        <v>5.533843994140625</v>
+        <v>37.488517488035733</v>
       </c>
       <c r="S7" s="3">
-        <v>5.4576892852783203</v>
+        <v>39.418748960193533</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -18874,58 +18868,58 @@
         <v>2016</v>
       </c>
       <c r="B8" s="3">
-        <v>5</v>
+        <v>60.353619475508992</v>
       </c>
       <c r="C8" s="3">
-        <v>5</v>
+        <v>60.954615467126899</v>
       </c>
       <c r="D8" s="3">
-        <v>5.0919504165649414</v>
+        <v>57.094903860118123</v>
       </c>
       <c r="E8" s="3">
-        <v>5.1979131698608398</v>
+        <v>57.564811685539411</v>
       </c>
       <c r="F8" s="3">
-        <v>5.2031617164611816</v>
+        <v>54.333622921988479</v>
       </c>
       <c r="G8" s="3">
-        <v>5.1261844635009766</v>
+        <v>55.494772969568302</v>
       </c>
       <c r="H8" s="3">
-        <v>5.1757388114929199</v>
+        <v>53.077178152767203</v>
       </c>
       <c r="I8" s="3">
-        <v>5.1646504402160636</v>
+        <v>54.48238978612595</v>
       </c>
       <c r="J8" s="3">
-        <v>5.0723490715026864</v>
+        <v>50.99080570198916</v>
       </c>
       <c r="K8" s="3">
-        <v>5.2336711883544922</v>
+        <v>52.751094072235837</v>
       </c>
       <c r="L8" s="3">
-        <v>5.0609664916992188</v>
+        <v>48.542738083565709</v>
       </c>
       <c r="M8" s="3">
-        <v>5.151423454284668</v>
+        <v>49.605959955612121</v>
       </c>
       <c r="N8" s="3">
-        <v>5.3805398941040039</v>
+        <v>46.142610622430787</v>
       </c>
       <c r="O8" s="3">
-        <v>5.3578758239746094</v>
+        <v>47.128155291476851</v>
       </c>
       <c r="P8" s="3">
-        <v>5.504906177520752</v>
+        <v>42.450699124394859</v>
       </c>
       <c r="Q8" s="3">
-        <v>5.5980491638183594</v>
+        <v>44.397583991917188</v>
       </c>
       <c r="R8" s="3">
-        <v>5.6329789161682129</v>
+        <v>37.524424307811387</v>
       </c>
       <c r="S8" s="3">
-        <v>5.525792121887207</v>
+        <v>39.84915810191756</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -18933,58 +18927,58 @@
         <v>2015</v>
       </c>
       <c r="B9" s="3">
-        <v>5</v>
+        <v>60.138571611488821</v>
       </c>
       <c r="C9" s="3">
-        <v>5</v>
+        <v>60.642514057769567</v>
       </c>
       <c r="D9" s="3">
-        <v>5.1161251068115234</v>
+        <v>56.89555439361969</v>
       </c>
       <c r="E9" s="3">
-        <v>5.1586780548095703</v>
+        <v>57.597302503673397</v>
       </c>
       <c r="F9" s="3">
-        <v>5.2322335243225098</v>
+        <v>54.601265437888003</v>
       </c>
       <c r="G9" s="3">
-        <v>5.0834388732910156</v>
+        <v>55.858637125374123</v>
       </c>
       <c r="H9" s="3">
-        <v>5.2577919960021973</v>
+        <v>53.070250358958369</v>
       </c>
       <c r="I9" s="3">
-        <v>5.1571202278137207</v>
+        <v>54.321014139721989</v>
       </c>
       <c r="J9" s="3">
-        <v>5.118781566619873</v>
+        <v>51.197581475806501</v>
       </c>
       <c r="K9" s="3">
-        <v>5.2070379257202148</v>
+        <v>52.645486514944231</v>
       </c>
       <c r="L9" s="3">
-        <v>5.0712604522705078</v>
+        <v>48.720476826273753</v>
       </c>
       <c r="M9" s="3">
-        <v>5.2050743103027344</v>
+        <v>50.198515086826717</v>
       </c>
       <c r="N9" s="3">
-        <v>5.4061694145202637</v>
+        <v>46.091826514558477</v>
       </c>
       <c r="O9" s="3">
-        <v>5.4122319221496582</v>
+        <v>47.225803882053803</v>
       </c>
       <c r="P9" s="3">
-        <v>5.6075849533081046</v>
+        <v>42.994746282706942</v>
       </c>
       <c r="Q9" s="3">
-        <v>5.5589408874511719</v>
+        <v>44.304782507942598</v>
       </c>
       <c r="R9" s="3">
-        <v>5.6058411598205566</v>
+        <v>37.893250863651851</v>
       </c>
       <c r="S9" s="3">
-        <v>5.5649847984313956</v>
+        <v>39.352172199681789</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -18992,58 +18986,58 @@
         <v>2014</v>
       </c>
       <c r="B10" s="3">
-        <v>5</v>
+        <v>59.831606697301211</v>
       </c>
       <c r="C10" s="3">
-        <v>5</v>
+        <v>60.40838619398663</v>
       </c>
       <c r="D10" s="3">
-        <v>5.0764522552490234</v>
+        <v>56.547492209419481</v>
       </c>
       <c r="E10" s="3">
-        <v>5.1371588706970206</v>
+        <v>57.10837087074983</v>
       </c>
       <c r="F10" s="3">
-        <v>5.1401801109313956</v>
+        <v>54.334526745312203</v>
       </c>
       <c r="G10" s="3">
-        <v>5.0399274826049796</v>
+        <v>55.555292223645409</v>
       </c>
       <c r="H10" s="3">
-        <v>5.1302390098571777</v>
+        <v>53.149158236566358</v>
       </c>
       <c r="I10" s="3">
-        <v>5.1695351600646973</v>
+        <v>54.257084619388003</v>
       </c>
       <c r="J10" s="3">
-        <v>5.013277530670166</v>
+        <v>51.353726772434847</v>
       </c>
       <c r="K10" s="3">
-        <v>5.0950078964233398</v>
+        <v>52.632467897088063</v>
       </c>
       <c r="L10" s="3">
-        <v>5.00811767578125</v>
+        <v>48.774476384309317</v>
       </c>
       <c r="M10" s="3">
-        <v>5.0053324699401864</v>
+        <v>50.066181742886549</v>
       </c>
       <c r="N10" s="3">
-        <v>5.240654468536377</v>
+        <v>45.950606838335823</v>
       </c>
       <c r="O10" s="3">
-        <v>5.2637662887573242</v>
+        <v>46.728700114406287</v>
       </c>
       <c r="P10" s="3">
-        <v>5.4207229614257813</v>
+        <v>42.636977887616432</v>
       </c>
       <c r="Q10" s="3">
-        <v>5.3660702705383301</v>
+        <v>43.902805168742383</v>
       </c>
       <c r="R10" s="3">
-        <v>5.4122648239135742</v>
+        <v>37.365107853917713</v>
       </c>
       <c r="S10" s="3">
-        <v>5.3903717994689941</v>
+        <v>39.518952871319449</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -19051,58 +19045,58 @@
         <v>2013</v>
       </c>
       <c r="B11" s="3">
-        <v>5</v>
+        <v>59.783508447303511</v>
       </c>
       <c r="C11" s="3">
-        <v>5</v>
+        <v>60.436915488348554</v>
       </c>
       <c r="D11" s="3">
-        <v>5.0274562835693359</v>
+        <v>56.829776664471439</v>
       </c>
       <c r="E11" s="3">
-        <v>5.1348271369934082</v>
+        <v>57.150289528515103</v>
       </c>
       <c r="F11" s="3">
-        <v>5.073122501373291</v>
+        <v>54.337327896295903</v>
       </c>
       <c r="G11" s="3">
-        <v>5.015228271484375</v>
+        <v>55.235208975054903</v>
       </c>
       <c r="H11" s="3">
-        <v>5.0312614440917969</v>
+        <v>53.472931022009817</v>
       </c>
       <c r="I11" s="3">
-        <v>5.018836498260498</v>
+        <v>54.317610288912768</v>
       </c>
       <c r="J11" s="3">
-        <v>4.8780503273010254</v>
+        <v>51.485480214747447</v>
       </c>
       <c r="K11" s="3">
-        <v>4.9120578765869141</v>
+        <v>52.754557462216731</v>
       </c>
       <c r="L11" s="3">
-        <v>4.7824912071228027</v>
+        <v>49.00095196342582</v>
       </c>
       <c r="M11" s="3">
-        <v>4.8404150009155273</v>
+        <v>50.006249458533937</v>
       </c>
       <c r="N11" s="3">
-        <v>5.2115879058837891</v>
+        <v>46.058320867747263</v>
       </c>
       <c r="O11" s="3">
-        <v>5.2317795753479004</v>
+        <v>47.23260953457747</v>
       </c>
       <c r="P11" s="3">
-        <v>5.2659387588500977</v>
+        <v>42.413534290768773</v>
       </c>
       <c r="Q11" s="3">
-        <v>5.2849340438842773</v>
+        <v>43.548990647552571</v>
       </c>
       <c r="R11" s="3">
-        <v>5.2209429740905762</v>
+        <v>37.631706410545661</v>
       </c>
       <c r="S11" s="3">
-        <v>5.2745275497436523</v>
+        <v>40.401702448873728</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -19110,58 +19104,58 @@
         <v>2012</v>
       </c>
       <c r="B12" s="3">
-        <v>5</v>
+        <v>59.720111431329322</v>
       </c>
       <c r="C12" s="3">
-        <v>5</v>
+        <v>60.426153372133207</v>
       </c>
       <c r="D12" s="3">
-        <v>5.0309200286865234</v>
+        <v>56.287818002928773</v>
       </c>
       <c r="E12" s="3">
-        <v>5.1089868545532227</v>
+        <v>57.02553251703246</v>
       </c>
       <c r="F12" s="3">
-        <v>5.0801091194152832</v>
+        <v>54.128384261371188</v>
       </c>
       <c r="G12" s="3">
-        <v>5.0289759635925293</v>
+        <v>55.175832994442217</v>
       </c>
       <c r="H12" s="3">
-        <v>5.1014132499694824</v>
+        <v>53.273057494314664</v>
       </c>
       <c r="I12" s="3">
-        <v>5.0315127372741699</v>
+        <v>54.078994391401977</v>
       </c>
       <c r="J12" s="3">
-        <v>4.940068244934082</v>
+        <v>51.678295107772357</v>
       </c>
       <c r="K12" s="3">
-        <v>4.9464812278747559</v>
+        <v>52.683593648897279</v>
       </c>
       <c r="L12" s="3">
-        <v>4.9116291999816886</v>
+        <v>49.02593647569568</v>
       </c>
       <c r="M12" s="3">
-        <v>4.9646220207214364</v>
+        <v>50.358925421940448</v>
       </c>
       <c r="N12" s="3">
-        <v>5.3228073120117188</v>
+        <v>46.343569742663597</v>
       </c>
       <c r="O12" s="3">
-        <v>5.2921652793884277</v>
+        <v>46.997701802793571</v>
       </c>
       <c r="P12" s="3">
-        <v>5.3400988578796387</v>
+        <v>42.311555511970496</v>
       </c>
       <c r="Q12" s="3">
-        <v>5.3663382530212402</v>
+        <v>44.079763540684063</v>
       </c>
       <c r="R12" s="3">
-        <v>5.2207603454589844</v>
+        <v>38.154248870243968</v>
       </c>
       <c r="S12" s="3">
-        <v>5.3171186447143546</v>
+        <v>40.839599545303862</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -19169,58 +19163,58 @@
         <v>2011</v>
       </c>
       <c r="B13" s="3">
-        <v>5</v>
+        <v>59.668692788581943</v>
       </c>
       <c r="C13" s="3">
-        <v>5</v>
+        <v>60.491844780602698</v>
       </c>
       <c r="D13" s="3">
-        <v>5.1176881790161133</v>
+        <v>56.433131239288443</v>
       </c>
       <c r="E13" s="3">
-        <v>5.167137622833252</v>
+        <v>57.157544062819973</v>
       </c>
       <c r="F13" s="3">
-        <v>5.156456470489502</v>
+        <v>54.432116597061267</v>
       </c>
       <c r="G13" s="3">
-        <v>5.1178812980651864</v>
+        <v>55.388803205042123</v>
       </c>
       <c r="H13" s="3">
-        <v>5.0922284126281738</v>
+        <v>53.513171015649952</v>
       </c>
       <c r="I13" s="3">
-        <v>5.0810575485229492</v>
+        <v>54.44162951266496</v>
       </c>
       <c r="J13" s="3">
-        <v>4.9971766471862793</v>
+        <v>51.604394488828213</v>
       </c>
       <c r="K13" s="3">
-        <v>5.0848617553710938</v>
+        <v>52.692942333289437</v>
       </c>
       <c r="L13" s="3">
-        <v>5.0091037750244141</v>
+        <v>48.823542187215999</v>
       </c>
       <c r="M13" s="3">
-        <v>5.0797119140625</v>
+        <v>49.982755911747191</v>
       </c>
       <c r="N13" s="3">
-        <v>5.37158203125</v>
+        <v>46.147637881215289</v>
       </c>
       <c r="O13" s="3">
-        <v>5.3439502716064453</v>
+        <v>46.895231410894162</v>
       </c>
       <c r="P13" s="3">
-        <v>5.4784607887268066</v>
+        <v>42.085259168606242</v>
       </c>
       <c r="Q13" s="3">
-        <v>5.4776649475097656</v>
+        <v>43.141845370236133</v>
       </c>
       <c r="R13" s="3">
-        <v>5.3830270767211914</v>
+        <v>37.575338617385214</v>
       </c>
       <c r="S13" s="3">
-        <v>5.4919390678405762</v>
+        <v>40.297658061501579</v>
       </c>
     </row>
   </sheetData>

</xml_diff>